<commit_message>
Modified Flower Configuration and Add SaveModelStrategy
</commit_message>
<xml_diff>
--- a/data/raw/ENERGY/labels.xlsx
+++ b/data/raw/ENERGY/labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimleang/Desktop/kl-dl-ml/tsad/data/raw/ENERGY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A21271-12B2-1644-B656-6F27CDE8C0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19861A1F-0EED-A74B-965C-E56AFE0BFE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="2480" windowWidth="27540" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="18200" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,8 +43,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -56,8 +63,20 @@
         <fgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -87,11 +106,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -104,6 +132,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,8 +168,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:A77" totalsRowShown="0">
-  <autoFilter ref="A1:A77" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:A103" totalsRowShown="0">
+  <autoFilter ref="A1:A103" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sample" totalsRowLabel="Total"/>
   </tableColumns>
@@ -419,10 +465,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -439,484 +485,614 @@
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+      <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="A30" s="6">
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+      <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+      <c r="A32" s="6">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+      <c r="A33" s="7">
         <v>284</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+      <c r="A34" s="6">
         <v>285</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+      <c r="A35" s="7">
         <v>286</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="A36" s="6">
         <v>287</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+      <c r="A37" s="7">
         <v>288</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="A38" s="6">
         <v>289</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+      <c r="A39" s="7">
         <v>290</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+      <c r="A40" s="6">
         <v>291</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
+      <c r="A41" s="7">
         <v>292</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
+      <c r="A42" s="6">
         <v>293</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
+      <c r="A43" s="7">
         <v>294</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+      <c r="A44" s="6">
         <v>295</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
     </row>
     <row r="45" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+      <c r="A45" s="7">
         <v>296</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+    <row r="46" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
         <v>297</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
+    <row r="47" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
         <v>298</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
+    <row r="48" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
         <v>299</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+    <row r="49" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
         <v>754</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
+    <row r="50" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8">
         <v>879</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
+    <row r="51" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
         <v>984</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
+    <row r="52" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="9">
         <v>3384</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="10">
         <v>3385</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="9">
         <v>3386</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="10">
         <v>3387</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="9">
         <v>3388</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="10">
         <v>3389</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="9">
         <v>3390</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="10">
         <v>3391</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="9">
         <v>3392</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="10">
         <v>3393</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="9">
         <v>3394</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="10">
         <v>3395</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="9">
         <v>3396</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="10">
         <v>3397</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="9">
         <v>3398</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="10">
         <v>3399</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="9">
         <v>3400</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="10">
         <v>3401</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="9">
         <v>3402</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="10">
         <v>3403</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="9">
         <v>3404</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="10">
         <v>3405</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="9">
         <v>3406</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="10">
         <v>3407</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="9">
         <v>3408</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="11">
         <v>3409</v>
       </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>